<commit_message>
git push origin master
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+  <si>
+    <t>상품번호</t>
+  </si>
   <si>
     <t>상품</t>
   </si>
@@ -22,130 +25,28 @@
     <t>가격</t>
   </si>
   <si>
-    <t>더블 백스트랩 오프숄더 브라탑(1855)</t>
+    <t>더블 백스트랩 오프숄더 브라탑</t>
   </si>
   <si>
     <t>블랙,스킨</t>
   </si>
   <si>
-    <t>소프트 프릴 크롭 브라탑(1439)</t>
+    <t>소프트 프릴 크롭 브라탑</t>
   </si>
   <si>
     <t>블랙,화이트</t>
   </si>
   <si>
-    <t>헤브 백리스 스트랩 브라렛(1861)</t>
+    <t>헤브 백리스 스트랩 브라렛</t>
   </si>
   <si>
-    <t>비비 백리스 나시 크롭탑(1869)</t>
+    <t>비비 백리스 나시 크롭탑</t>
   </si>
   <si>
-    <t>원썸 홀터넥 브라탑(1871)</t>
+    <t>원썸 홀터넥 브라탑</t>
   </si>
   <si>
-    <t>옆셔링 스퀘어 나시탑(1873)</t>
-  </si>
-  <si>
-    <t>퓨어 골지 나시탑(1879)</t>
-  </si>
-  <si>
-    <t>화이트,핑크,그레이,블랙</t>
-  </si>
-  <si>
-    <t>폭신 끈나시 크롭 브라탑(1864)</t>
-  </si>
-  <si>
-    <t>슬림핏 크롭 끈나시(1266)</t>
-  </si>
-  <si>
-    <t>스트라이프 버튼 크롭 캡나시(1984)</t>
-  </si>
-  <si>
-    <t>오비어스 레터링 배색 캡나시(1989)</t>
-  </si>
-  <si>
-    <t>화이트,네이비</t>
-  </si>
-  <si>
-    <t>레이스 버튼 슬림핏 캡나시(1985)</t>
-  </si>
-  <si>
-    <t>리즈 레이스 브이넥 캡나시(1986)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 뮤뮤 레이스 캡나시 (1990)</t>
-  </si>
-  <si>
-    <t>화이트,그레이,블랙</t>
-  </si>
-  <si>
-    <t>뮤디 파스텔 캡나시(1894)</t>
-  </si>
-  <si>
-    <t>화이트,핑크,그린,스카이,그레이,블랙</t>
-  </si>
-  <si>
-    <t>프린 레이스 크롭 브라렛(1264)</t>
-  </si>
-  <si>
-    <t>프릴 셔링 브라탑(1878)</t>
-  </si>
-  <si>
-    <t>라인 백리스 끈 홀터넥 브라탑(1870)</t>
-  </si>
-  <si>
-    <t>꼬임 셔링 브라탑(1865)</t>
-  </si>
-  <si>
-    <t>탄탄 오프숄더 튜브탑(1435)</t>
-  </si>
-  <si>
-    <t>더블후크 오프숄더 브라탑 (1857)</t>
-  </si>
-  <si>
-    <t>글램 크로스 백 골지 브라탑(1856)</t>
-  </si>
-  <si>
-    <t>쫀쫀 골지 브라렛 세트(1429)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 엑스끈 브이넥 밍크 캡 나시(2345)</t>
-  </si>
-  <si>
-    <t>스킨,그레이,블랙</t>
-  </si>
-  <si>
-    <t>스퀘어넥 밍크 캡 나시(2346)</t>
-  </si>
-  <si>
-    <t>스노우 양기모 캡나시(2343)</t>
-  </si>
-  <si>
-    <t>아이보리,블랙</t>
-  </si>
-  <si>
-    <t>위드 밍크 기모 캡나시(2344)</t>
-  </si>
-  <si>
-    <t>엠마 골지 밍크 기모 캡나시 (2347)</t>
-  </si>
-  <si>
-    <t>블랙,크림베이지</t>
-  </si>
-  <si>
-    <t>스퀘어 골지 기모 크롭 캡나시(2342)</t>
-  </si>
-  <si>
-    <t>더블 스트랩 밍크 기모 캡나시(2341)</t>
-  </si>
-  <si>
-    <t>양기모 캡나시 (2406)</t>
-  </si>
-  <si>
-    <t>베이지,차콜,블랙</t>
-  </si>
-  <si>
-    <t>체인 스트랩 골지 크롭탑(1866)</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -209,9 +110,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -437,480 +341,216 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="40.71"/>
-    <col customWidth="1" min="3" max="3" width="18.57"/>
-    <col customWidth="1" min="4" max="4" width="16.71"/>
-    <col customWidth="1" min="5" max="17" width="8.71"/>
+    <col customWidth="1" min="1" max="2" width="8.71"/>
+    <col customWidth="1" min="3" max="3" width="40.71"/>
+    <col customWidth="1" min="4" max="4" width="18.57"/>
+    <col customWidth="1" min="5" max="5" width="16.71"/>
+    <col customWidth="1" min="6" max="18" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" ht="16.5" customHeight="1">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>1.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+      <c r="B2" s="1">
+        <v>1234.0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3">
         <v>1300.0</v>
       </c>
     </row>
     <row r="3" ht="16.5" customHeight="1">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>2.0</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>1235.0</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3">
         <v>2900.0</v>
       </c>
     </row>
     <row r="4" ht="16.5" customHeight="1">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>3.0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="1">
+        <v>2346.0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="E4" s="3">
         <v>3500.0</v>
       </c>
     </row>
     <row r="5" ht="16.5" customHeight="1">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>4.0</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
+      <c r="B5" s="1">
+        <v>734.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3">
         <v>2800.0</v>
       </c>
     </row>
     <row r="6" ht="16.5" customHeight="1">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>5.0</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
+      <c r="B6" s="1">
+        <v>3344.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3">
         <v>2600.0</v>
       </c>
     </row>
     <row r="7" ht="16.5" customHeight="1">
-      <c r="A7" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2700.0</v>
-      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" ht="16.5" customHeight="1">
-      <c r="A8" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" ht="16.5" customHeight="1">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" ht="16.5" customHeight="1">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" ht="16.5" customHeight="1">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" ht="16.5" customHeight="1">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" ht="16.5" customHeight="1">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" ht="16.5" customHeight="1">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" ht="16.5" customHeight="1">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" ht="16.5" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" ht="16.5" customHeight="1">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" ht="16.5" customHeight="1">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" ht="16.5" customHeight="1">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" ht="16.5" customHeight="1">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" ht="16.5" customHeight="1">
+      <c r="E21" s="3"/>
+      <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2">
-        <v>3900.0</v>
-      </c>
-    </row>
-    <row r="9" ht="16.5" customHeight="1">
-      <c r="A9" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1900.0</v>
-      </c>
-    </row>
-    <row r="10" ht="16.5" customHeight="1">
-      <c r="A10" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2">
-        <v>2900.0</v>
-      </c>
-    </row>
-    <row r="11" ht="16.5" customHeight="1">
-      <c r="A11" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="2">
-        <v>4600.0</v>
-      </c>
-    </row>
-    <row r="12" ht="16.5" customHeight="1">
-      <c r="A12" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2600.0</v>
-      </c>
-    </row>
-    <row r="13" ht="16.5" customHeight="1">
-      <c r="A13" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="2">
-        <v>3600.0</v>
-      </c>
-    </row>
-    <row r="14" ht="16.5" customHeight="1">
-      <c r="A14" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2">
-        <v>4500.0</v>
-      </c>
-    </row>
-    <row r="15" ht="16.5" customHeight="1">
-      <c r="A15" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="2">
-        <v>4900.0</v>
-      </c>
-    </row>
-    <row r="16" ht="16.5" customHeight="1">
-      <c r="A16" s="4">
-        <v>15.0</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="5">
-        <v>3400.0</v>
-      </c>
-    </row>
-    <row r="17" ht="16.5" customHeight="1">
-      <c r="A17" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="2">
-        <v>3200.0</v>
-      </c>
-    </row>
-    <row r="18" ht="16.5" customHeight="1">
-      <c r="A18" s="1">
-        <v>17.0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="2">
-        <v>4300.0</v>
-      </c>
-    </row>
-    <row r="19" ht="16.5" customHeight="1">
-      <c r="A19" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="2">
-        <v>2200.0</v>
-      </c>
-    </row>
-    <row r="20" ht="16.5" customHeight="1">
-      <c r="A20" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="2">
-        <v>2700.0</v>
-      </c>
-    </row>
-    <row r="21" ht="16.5" customHeight="1">
-      <c r="A21" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="2">
-        <v>3600.0</v>
-      </c>
     </row>
     <row r="22" ht="16.5" customHeight="1">
-      <c r="A22" s="1">
-        <v>21.0</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="2">
-        <v>2900.0</v>
-      </c>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" ht="16.5" customHeight="1">
-      <c r="A23" s="1">
-        <v>22.0</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="2">
-        <v>1900.0</v>
-      </c>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" ht="16.5" customHeight="1">
-      <c r="A24" s="1">
-        <v>23.0</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="2">
-        <v>3600.0</v>
-      </c>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" ht="16.5" customHeight="1">
-      <c r="A25" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="2">
-        <v>3600.0</v>
-      </c>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" ht="16.5" customHeight="1">
-      <c r="A26" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="2">
-        <v>2900.0</v>
-      </c>
+      <c r="E26" s="3"/>
     </row>
     <row r="27" ht="16.5" customHeight="1">
-      <c r="A27" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="2">
-        <v>5900.0</v>
-      </c>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" ht="16.5" customHeight="1">
-      <c r="A28" s="1">
-        <v>27.0</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="2">
-        <v>3300.0</v>
-      </c>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" ht="16.5" customHeight="1">
-      <c r="A29" s="1">
-        <v>28.0</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="2">
-        <v>6200.0</v>
-      </c>
+      <c r="E29" s="3"/>
     </row>
     <row r="30" ht="16.5" customHeight="1">
-      <c r="A30" s="1">
-        <v>29.0</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="2">
-        <v>5500.0</v>
-      </c>
+      <c r="E30" s="3"/>
     </row>
     <row r="31" ht="16.5" customHeight="1">
-      <c r="A31" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="2">
-        <v>5900.0</v>
-      </c>
+      <c r="E31" s="3"/>
     </row>
     <row r="32" ht="16.5" customHeight="1">
-      <c r="A32" s="1">
-        <v>31.0</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="2">
-        <v>5400.0</v>
-      </c>
+      <c r="E32" s="3"/>
     </row>
     <row r="33" ht="16.5" customHeight="1">
-      <c r="A33" s="6">
-        <v>32.0</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
     </row>
     <row r="34" ht="16.5" customHeight="1"/>
     <row r="35" ht="16.5" customHeight="1"/>

</xml_diff>